<commit_message>
Fancybox pagina gemaakt, nieuwe planning toegevoed. Web.config aanpassen
</commit_message>
<xml_diff>
--- a/Documentatie/Planning/Planning Milanov 2013.xlsx
+++ b/Documentatie/Planning/Planning Milanov 2013.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Planning  Milanov P3P</t>
   </si>
@@ -79,6 +79,69 @@
   </si>
   <si>
     <t>Perfectioneren</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Wat</t>
+  </si>
+  <si>
+    <t>Wie</t>
+  </si>
+  <si>
+    <t>Yme, Wouter, Niek</t>
+  </si>
+  <si>
+    <t>Design FrontEnd</t>
+  </si>
+  <si>
+    <t>Yme, Wouter</t>
+  </si>
+  <si>
+    <t>Design BackEnd</t>
+  </si>
+  <si>
+    <t>Niek</t>
+  </si>
+  <si>
+    <t>Yme</t>
+  </si>
+  <si>
+    <t>CMS Systeem</t>
+  </si>
+  <si>
+    <t>Yme,Wouter,Niek</t>
+  </si>
+  <si>
+    <t>Database aanmaken</t>
+  </si>
+  <si>
+    <t>Yme,Wouter</t>
+  </si>
+  <si>
+    <t>Betaling</t>
+  </si>
+  <si>
+    <t>Login/Register</t>
+  </si>
+  <si>
+    <t>Yme,Niek</t>
+  </si>
+  <si>
+    <t>Wouter</t>
+  </si>
+  <si>
+    <t>Taakverdeling</t>
   </si>
 </sst>
 </file>
@@ -213,27 +276,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -242,9 +293,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,6 +306,81 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -562,385 +685,645 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5">
         <v>6</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>7</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="5">
         <v>8</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="5">
         <v>9</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="5">
         <v>10</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="5">
         <v>11</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="5">
         <v>12</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="5">
         <v>13</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="13"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="18"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="41"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="26"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="22"/>
+    </row>
+    <row r="16" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="18"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="41"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="41"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="41"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="41"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="19"/>
-      <c r="D23" s="2" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="14"/>
+      <c r="D28" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="2" t="s">
+      <c r="E28" s="36"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="2" t="s">
+      <c r="H28" s="36"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K28" s="36"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="28"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="27"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="27"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="27"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="27"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="27"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="27"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
+  <mergeCells count="72">
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="M19:N19"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="G20:M20"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="M18:N18"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="A9:D9"/>
@@ -948,14 +1331,66 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="K10:N10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="G25:M25"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B46:D46"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:N7 A17:N19 A8:F9 H8:N8 A10:H10 J10:K10 A11:K11 L12 A12:J13 L13:M13 A14:M14 A15:L16 A20:G20 N20">
+  <conditionalFormatting sqref="A6:N7 A15:A17 A22:N24 A8:F9 H8:N8 A10:H10 J10:K11 A12:K12 L13:L17 A13:J13 L18:M18 A19:M19 A20:L21 A25:G25 N25 A18:J18 E14:J17 A11 E11:H11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -976,11 +1411,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>